<commit_message>
Adding data fro phase 1 and updated rows 70-100 to not include Serbian characters
</commit_message>
<xml_diff>
--- a/upiti.xlsx
+++ b/upiti.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jokan\Documents\LENA\Masters\OPJ\natural-language-processing-project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DED02E3-A565-47D2-8BD7-20B420D20E06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upiti" sheetId="1" r:id="rId1"/>
@@ -133,9 +139,6 @@
     <t>jedinstveni elementi</t>
   </si>
   <si>
-    <t>??toplotna mapa 3D koordinata</t>
-  </si>
-  <si>
     <t>kako ekstraktovati zip fajl rekurzivno</t>
   </si>
   <si>
@@ -148,9 +151,6 @@
     <t>konvertuj datuma u obliku stringa u oblik ggggmmdd</t>
   </si>
   <si>
-    <t>konvertuj utc vremena u ??epoh vreme</t>
-  </si>
-  <si>
     <t>sve permutacije liste</t>
   </si>
   <si>
@@ -184,9 +184,6 @@
     <t>parsiraj string upit u url-a</t>
   </si>
   <si>
-    <t>??fuzzy match ranking</t>
-  </si>
-  <si>
     <t>izlaz html fajla</t>
   </si>
   <si>
@@ -247,36 +244,15 @@
     <t>baferovan fajl čitač čita tekst</t>
   </si>
   <si>
-    <t>množenje matrica</t>
-  </si>
-  <si>
-    <t>ekstrakcija podatka iz html sadržaja</t>
-  </si>
-  <si>
-    <t>uzeti sve roditelje od xml čvora</t>
-  </si>
-  <si>
-    <t>podvući tekst u nazivu vidžeta</t>
-  </si>
-  <si>
     <t>kopiranje fajla u određenu putanju</t>
   </si>
   <si>
     <t>nasumično ekstrahovati iks elemenata iz liste</t>
   </si>
   <si>
-    <t>kako čitati .csv fajl na efikasan način?</t>
-  </si>
-  <si>
     <t>čitanje elemenata from html-a &lt;td&gt;</t>
   </si>
   <si>
-    <t>kako citati sadržaj .gz kompresovanog fajla?</t>
-  </si>
-  <si>
-    <t>pamćenje na disku - stalno skladište</t>
-  </si>
-  <si>
     <t>konvertuj celobrojnu vrednost u string</t>
   </si>
   <si>
@@ -314,13 +290,43 @@
   </si>
   <si>
     <t>parsiranje json fajla</t>
+  </si>
+  <si>
+    <t>fuzzy match ranking</t>
+  </si>
+  <si>
+    <t>konvertuj utc vremena u epoh vreme</t>
+  </si>
+  <si>
+    <t>toplotna mapa 3D koordinata</t>
+  </si>
+  <si>
+    <t>ekstrakcija podatka iz html sadrzaja</t>
+  </si>
+  <si>
+    <t>uzeti sve roditelje od xml cvora</t>
+  </si>
+  <si>
+    <t>podvući tekst u nazivu vidzeta</t>
+  </si>
+  <si>
+    <t>pamcenje na disku - stalno skladiste</t>
+  </si>
+  <si>
+    <t>kako citati sadrzaj .gz kompresovanog fajla?</t>
+  </si>
+  <si>
+    <t>kako čitati .csv fajl na efikasan nacin?</t>
+  </si>
+  <si>
+    <t>mnozenje matrica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -847,6 +853,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -893,7 +907,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -925,9 +939,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -959,6 +991,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1134,516 +1184,516 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
-      <c r="A81" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
-      <c r="A84" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
-      <c r="A85" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
-      <c r="A86" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
-      <c r="A87" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
-      <c r="A88" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
-      <c r="A92" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
-      <c r="A94" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Lena's faza_2.xlsx and some modifications in upiti.xlsx
</commit_message>
<xml_diff>
--- a/upiti.xlsx
+++ b/upiti.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jokan\Documents\LENA\Masters\OPJ\natural-language-processing-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DED02E3-A565-47D2-8BD7-20B420D20E06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D6AA63-4B44-4D5F-9254-3DFB4D9DC8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,30 +160,18 @@
     <t>kako proveriti da li je polje za potvrdu selektovano</t>
   </si>
   <si>
-    <t>konverzija uint8 niza u sliku</t>
-  </si>
-  <si>
     <t>parsiranja argumenata sa komandne linije</t>
   </si>
   <si>
     <t>slanje binarnog podataka preko serijske konekcije</t>
   </si>
   <si>
-    <t>ekstrahovanje podataka iz tekstualnog fajla</t>
-  </si>
-  <si>
-    <t>pozicija pod stringova u string</t>
-  </si>
-  <si>
     <t>oduzimanje srednje vrednosti od svake kolone</t>
   </si>
   <si>
     <t>nadovezi nekoliko fajlova izbrisi linije zaglavlja</t>
   </si>
   <si>
-    <t>parsiraj string upit u url-a</t>
-  </si>
-  <si>
     <t>izlaz html fajla</t>
   </si>
   <si>
@@ -244,15 +232,9 @@
     <t>baferovan fajl čitač čita tekst</t>
   </si>
   <si>
-    <t>kopiranje fajla u određenu putanju</t>
-  </si>
-  <si>
     <t>nasumično ekstrahovati iks elemenata iz liste</t>
   </si>
   <si>
-    <t>čitanje elemenata from html-a &lt;td&gt;</t>
-  </si>
-  <si>
     <t>konvertuj celobrojnu vrednost u string</t>
   </si>
   <si>
@@ -301,25 +283,43 @@
     <t>toplotna mapa 3D koordinata</t>
   </si>
   <si>
-    <t>ekstrakcija podatka iz html sadrzaja</t>
-  </si>
-  <si>
     <t>uzeti sve roditelje od xml cvora</t>
   </si>
   <si>
-    <t>podvući tekst u nazivu vidzeta</t>
-  </si>
-  <si>
     <t>pamcenje na disku - stalno skladiste</t>
   </si>
   <si>
-    <t>kako citati sadrzaj .gz kompresovanog fajla?</t>
-  </si>
-  <si>
-    <t>kako čitati .csv fajl na efikasan nacin?</t>
-  </si>
-  <si>
     <t>mnozenje matrica</t>
+  </si>
+  <si>
+    <t>ekstrakcija podataka iz html sadrzaja</t>
+  </si>
+  <si>
+    <t>podvuci tekst u nazivu vidzeta</t>
+  </si>
+  <si>
+    <t>kopiranje fajla u odredjenu putanju</t>
+  </si>
+  <si>
+    <t>konverzija uin8 niza u sliku</t>
+  </si>
+  <si>
+    <t>kako citati sadrzaj .gz kompresovanog fajla</t>
+  </si>
+  <si>
+    <t>ekstrakcija podataka iz tekstualnog fajla</t>
+  </si>
+  <si>
+    <t>pozicija pod stringova u stringu</t>
+  </si>
+  <si>
+    <t>citanje elemenata from html-a &lt;td&gt;</t>
+  </si>
+  <si>
+    <t>parsiraj string upit u urla</t>
+  </si>
+  <si>
+    <t>kako citati .csv fajl na efikasan nacin</t>
   </si>
 </sst>
 </file>
@@ -1187,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -1223,17 +1223,17 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -1243,7 +1243,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
@@ -1263,17 +1263,17 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -1303,12 +1303,12 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
@@ -1318,12 +1318,12 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
@@ -1338,42 +1338,42 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
@@ -1383,12 +1383,12 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -1403,7 +1403,7 @@
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
@@ -1438,7 +1438,7 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
@@ -1453,7 +1453,7 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
@@ -1468,7 +1468,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
@@ -1483,7 +1483,7 @@
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
@@ -1493,7 +1493,7 @@
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
@@ -1503,7 +1503,7 @@
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
@@ -1518,12 +1518,12 @@
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
@@ -1533,7 +1533,7 @@
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
@@ -1543,7 +1543,7 @@
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
@@ -1558,17 +1558,17 @@
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
@@ -1578,7 +1578,7 @@
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
@@ -1588,7 +1588,7 @@
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
@@ -1598,7 +1598,7 @@
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
@@ -1608,7 +1608,7 @@
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
@@ -1628,72 +1628,72 @@
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>